<commit_message>
fix tải các bảng công CHủ Nhật
</commit_message>
<xml_diff>
--- a/static/uploads/mau/bangcong/mau_bangchamcong_chitiet_chunhat_chot.xlsx
+++ b/static/uploads/mau/bangcong/mau_bangchamcong_chitiet_chunhat_chot.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DAT\Desktop\code\working\HRM\static\uploads\mau\bangcong\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ACFAE6B-F3B6-49D2-A548-55D39EB8A799}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58BBC7B-403F-46E5-A53F-388F9198105C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Nhà máy</t>
   </si>
@@ -37,18 +37,12 @@
     <t>Chức danh</t>
   </si>
   <si>
-    <t>Cấp bậc</t>
-  </si>
-  <si>
     <t>Ngày</t>
   </si>
   <si>
     <t>Ca</t>
   </si>
   <si>
-    <t>Số phút ca</t>
-  </si>
-  <si>
     <t>Giờ vào</t>
   </si>
   <si>
@@ -58,37 +52,19 @@
     <t>Phút hành chính</t>
   </si>
   <si>
-    <t>Phút nghỉ phép</t>
-  </si>
-  <si>
-    <t>Phút tăng ca 100%</t>
-  </si>
-  <si>
-    <t>Phút tăng ca 150%</t>
-  </si>
-  <si>
-    <t>Phút nghỉ không lương</t>
-  </si>
-  <si>
     <t>Phút nghỉ khác</t>
   </si>
   <si>
     <t>Loại nghỉ khác</t>
   </si>
   <si>
-    <t>Phân loại</t>
-  </si>
-  <si>
     <t>Phòng ban</t>
   </si>
   <si>
-    <t>HC Category</t>
-  </si>
-  <si>
-    <t>Phút tăng ca đêm</t>
-  </si>
-  <si>
     <t>BẢNG CHẤM CÔNG CHI TIẾT CHỦ NHẬT CHỐT</t>
+  </si>
+  <si>
+    <t>Phút tăng ca 200%</t>
   </si>
 </sst>
 </file>
@@ -504,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AQ3"/>
+  <dimension ref="A1:AI3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:U2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,25 +494,18 @@
     <col min="4" max="4" width="25.7109375" customWidth="1"/>
     <col min="5" max="5" width="10.5703125" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="9" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" customWidth="1"/>
-    <col min="9" max="9" width="7" customWidth="1"/>
-    <col min="10" max="10" width="12" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" customWidth="1"/>
-    <col min="12" max="12" width="8" customWidth="1"/>
-    <col min="13" max="13" width="17" customWidth="1"/>
-    <col min="14" max="14" width="16" customWidth="1"/>
-    <col min="15" max="16" width="19" customWidth="1"/>
-    <col min="17" max="17" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23" customWidth="1"/>
-    <col min="19" max="20" width="16" customWidth="1"/>
-    <col min="21" max="21" width="12" customWidth="1"/>
-    <col min="22" max="22" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
+    <col min="8" max="8" width="7" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" customWidth="1"/>
+    <col min="10" max="10" width="8" customWidth="1"/>
+    <col min="11" max="11" width="17" customWidth="1"/>
+    <col min="12" max="12" width="19" customWidth="1"/>
+    <col min="13" max="14" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -551,20 +520,13 @@
       <c r="L1" s="7"/>
       <c r="M1" s="7"/>
       <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7"/>
-      <c r="U1" s="7"/>
-      <c r="AM1" s="3"/>
-      <c r="AN1" s="3"/>
-      <c r="AO1" s="3"/>
-      <c r="AP1" s="4"/>
-      <c r="AQ1" s="4"/>
+      <c r="AE1" s="3"/>
+      <c r="AF1" s="3"/>
+      <c r="AG1" s="3"/>
+      <c r="AH1" s="4"/>
+      <c r="AI1" s="4"/>
     </row>
-    <row r="2" spans="1:43" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -579,20 +541,13 @@
       <c r="L2" s="8"/>
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="8"/>
-      <c r="AM2" s="5"/>
-      <c r="AN2" s="5"/>
-      <c r="AO2" s="5"/>
-      <c r="AP2" s="6"/>
-      <c r="AQ2" s="6"/>
+      <c r="AE2" s="5"/>
+      <c r="AF2" s="5"/>
+      <c r="AG2" s="5"/>
+      <c r="AH2" s="6"/>
+      <c r="AI2" s="6"/>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -609,12 +564,12 @@
         <v>3</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="I3" s="1" t="s">
@@ -627,43 +582,19 @@
         <v>9</v>
       </c>
       <c r="L3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:U1"/>
-    <mergeCell ref="A2:U2"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="A2:N2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
bỏ cột Phút HC các bảng công Chủ nhật
</commit_message>
<xml_diff>
--- a/static/uploads/mau/bangcong/mau_bangchamcong_chitiet_chunhat_chot.xlsx
+++ b/static/uploads/mau/bangcong/mau_bangchamcong_chitiet_chunhat_chot.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DAT\Desktop\code\working\HRM\static\uploads\mau\bangcong\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58BBC7B-403F-46E5-A53F-388F9198105C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8902423-0C6B-41E1-A104-351728326BAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Nhà máy</t>
   </si>
@@ -47,9 +47,6 @@
   </si>
   <si>
     <t>Giờ ra</t>
-  </si>
-  <si>
-    <t>Phút hành chính</t>
   </si>
   <si>
     <t>Phút nghỉ khác</t>
@@ -480,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AI3"/>
+  <dimension ref="A1:AH3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I1:I1048576"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,14 +495,13 @@
     <col min="8" max="8" width="7" customWidth="1"/>
     <col min="9" max="9" width="9.140625" customWidth="1"/>
     <col min="10" max="10" width="8" customWidth="1"/>
-    <col min="11" max="11" width="17" customWidth="1"/>
-    <col min="12" max="12" width="19" customWidth="1"/>
-    <col min="13" max="14" width="16" customWidth="1"/>
+    <col min="11" max="11" width="19" customWidth="1"/>
+    <col min="12" max="13" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -519,14 +515,13 @@
       <c r="K1" s="7"/>
       <c r="L1" s="7"/>
       <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
+      <c r="AD1" s="3"/>
       <c r="AE1" s="3"/>
       <c r="AF1" s="3"/>
-      <c r="AG1" s="3"/>
+      <c r="AG1" s="4"/>
       <c r="AH1" s="4"/>
-      <c r="AI1" s="4"/>
     </row>
-    <row r="2" spans="1:35" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -540,14 +535,13 @@
       <c r="K2" s="8"/>
       <c r="L2" s="8"/>
       <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
+      <c r="AD2" s="5"/>
       <c r="AE2" s="5"/>
       <c r="AF2" s="5"/>
-      <c r="AG2" s="5"/>
+      <c r="AG2" s="6"/>
       <c r="AH2" s="6"/>
-      <c r="AI2" s="6"/>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -564,7 +558,7 @@
         <v>3</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>5</v>
@@ -579,22 +573,19 @@
         <v>8</v>
       </c>
       <c r="K3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="A2:N2"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A2:M2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>